<commit_message>
[add] - 60% accuracy model
</commit_message>
<xml_diff>
--- a/temp_submit/COBRE_test_brain_age_submission_소융과_2020105695_김희성_6_12.xlsx
+++ b/temp_submit/COBRE_test_brain_age_submission_소융과_2020105695_김희성_6_12.xlsx
@@ -355,7 +355,7 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -376,7 +376,7 @@
         <v>40000</v>
       </c>
       <c r="B2" s="1">
-        <v>42.308140000000002</v>
+        <v>40.100853000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -384,7 +384,7 @@
         <v>40001</v>
       </c>
       <c r="B3" s="1">
-        <v>45.828180000000003</v>
+        <v>39.946536999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -392,7 +392,7 @@
         <v>40002</v>
       </c>
       <c r="B4" s="1">
-        <v>37.024754000000001</v>
+        <v>40.53078</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -400,7 +400,7 @@
         <v>40003</v>
       </c>
       <c r="B5" s="1">
-        <v>49.303699999999999</v>
+        <v>44.958874000000002</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -408,7 +408,7 @@
         <v>40004</v>
       </c>
       <c r="B6" s="1">
-        <v>40.704796000000002</v>
+        <v>43.621464000000003</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -416,7 +416,7 @@
         <v>40005</v>
       </c>
       <c r="B7" s="1">
-        <v>42.221404999999997</v>
+        <v>36.777602999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -424,7 +424,7 @@
         <v>40006</v>
       </c>
       <c r="B8" s="1">
-        <v>35.232613000000001</v>
+        <v>46.88138</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -432,7 +432,7 @@
         <v>40007</v>
       </c>
       <c r="B9" s="1">
-        <v>49.800021999999998</v>
+        <v>37.578800000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -440,7 +440,7 @@
         <v>40008</v>
       </c>
       <c r="B10" s="1">
-        <v>40.639713</v>
+        <v>43.728610000000003</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -448,7 +448,7 @@
         <v>40009</v>
       </c>
       <c r="B11" s="1">
-        <v>39.073543999999998</v>
+        <v>39.494340000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -456,7 +456,7 @@
         <v>40010</v>
       </c>
       <c r="B12" s="1">
-        <v>44.625830000000001</v>
+        <v>54.792225000000002</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -464,7 +464,7 @@
         <v>40011</v>
       </c>
       <c r="B13" s="1">
-        <v>38.542724999999997</v>
+        <v>43.195410000000003</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -472,7 +472,7 @@
         <v>40012</v>
       </c>
       <c r="B14" s="1">
-        <v>38.219560000000001</v>
+        <v>35.122239999999998</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -480,7 +480,7 @@
         <v>40015</v>
       </c>
       <c r="B15" s="1">
-        <v>41.846767</v>
+        <v>47.962739999999997</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -488,7 +488,7 @@
         <v>40016</v>
       </c>
       <c r="B16" s="1">
-        <v>42.619945999999999</v>
+        <v>41.124786</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -496,7 +496,7 @@
         <v>40021</v>
       </c>
       <c r="B17" s="1">
-        <v>42.153919999999999</v>
+        <v>50.208480000000002</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -504,7 +504,7 @@
         <v>40022</v>
       </c>
       <c r="B18" s="1">
-        <v>39.03389</v>
+        <v>40.018830000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -512,7 +512,7 @@
         <v>40025</v>
       </c>
       <c r="B19" s="1">
-        <v>38.883434000000001</v>
+        <v>38.292313</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
@@ -520,7 +520,7 @@
         <v>40028</v>
       </c>
       <c r="B20" s="1">
-        <v>37.222614</v>
+        <v>49.403060000000004</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
@@ -528,7 +528,7 @@
         <v>40029</v>
       </c>
       <c r="B21" s="1">
-        <v>40.612609999999997</v>
+        <v>43.034443000000003</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
@@ -536,7 +536,7 @@
         <v>40032</v>
       </c>
       <c r="B22" s="1">
-        <v>39.763460000000002</v>
+        <v>44.354393000000002</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
@@ -544,7 +544,7 @@
         <v>40034</v>
       </c>
       <c r="B23" s="1">
-        <v>51.123047</v>
+        <v>36.866250000000001</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -552,7 +552,7 @@
         <v>40037</v>
       </c>
       <c r="B24" s="1">
-        <v>51.837226999999999</v>
+        <v>42.497272000000002</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -560,7 +560,7 @@
         <v>40039</v>
       </c>
       <c r="B25" s="1">
-        <v>39.129204000000001</v>
+        <v>43.42118</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
@@ -568,7 +568,7 @@
         <v>40040</v>
       </c>
       <c r="B26" s="1">
-        <v>40.348132999999997</v>
+        <v>35.680250000000001</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
@@ -576,7 +576,7 @@
         <v>40041</v>
       </c>
       <c r="B27" s="1">
-        <v>46.885680000000001</v>
+        <v>49.568171999999997</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
@@ -584,7 +584,7 @@
         <v>40042</v>
       </c>
       <c r="B28" s="1">
-        <v>42.678759999999997</v>
+        <v>36.556429999999999</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -592,7 +592,7 @@
         <v>40044</v>
       </c>
       <c r="B29" s="1">
-        <v>43.103766999999998</v>
+        <v>44.58229</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
@@ -600,7 +600,7 @@
         <v>40046</v>
       </c>
       <c r="B30" s="1">
-        <v>39.961964000000002</v>
+        <v>45.114086</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -608,7 +608,7 @@
         <v>40047</v>
       </c>
       <c r="B31" s="1">
-        <v>39.146915</v>
+        <v>33.393639999999998</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
@@ -616,7 +616,7 @@
         <v>40049</v>
       </c>
       <c r="B32" s="1">
-        <v>42.13167</v>
+        <v>46.05442</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
@@ -624,7 +624,7 @@
         <v>40059</v>
       </c>
       <c r="B33" s="1">
-        <v>46.877357000000003</v>
+        <v>35.413902</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
@@ -632,7 +632,7 @@
         <v>40060</v>
       </c>
       <c r="B34" s="1">
-        <v>41.190703999999997</v>
+        <v>37.274470000000001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -640,7 +640,7 @@
         <v>40064</v>
       </c>
       <c r="B35" s="1">
-        <v>37.197353</v>
+        <v>42.358919999999998</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -648,7 +648,7 @@
         <v>40071</v>
       </c>
       <c r="B36" s="1">
-        <v>35.14593</v>
+        <v>42.065849999999998</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -656,7 +656,7 @@
         <v>40072</v>
       </c>
       <c r="B37" s="1">
-        <v>45.810307000000002</v>
+        <v>42.880443999999997</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -664,7 +664,7 @@
         <v>40073</v>
       </c>
       <c r="B38" s="1">
-        <v>42.580550000000002</v>
+        <v>39.902287000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -672,7 +672,7 @@
         <v>40075</v>
       </c>
       <c r="B39" s="1">
-        <v>45.661068</v>
+        <v>41.349105999999999</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -680,7 +680,7 @@
         <v>40077</v>
       </c>
       <c r="B40" s="1">
-        <v>39.551242999999999</v>
+        <v>39.446002999999997</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -688,7 +688,7 @@
         <v>40078</v>
       </c>
       <c r="B41" s="1">
-        <v>41.961734999999997</v>
+        <v>39.282955000000001</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -696,7 +696,7 @@
         <v>40079</v>
       </c>
       <c r="B42" s="1">
-        <v>41.064239999999998</v>
+        <v>44.553513000000002</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -704,7 +704,7 @@
         <v>40080</v>
       </c>
       <c r="B43" s="1">
-        <v>47.852406000000002</v>
+        <v>42.507862000000003</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -712,7 +712,7 @@
         <v>40081</v>
       </c>
       <c r="B44" s="1">
-        <v>54.969555</v>
+        <v>36.455886999999997</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
@@ -720,7 +720,7 @@
         <v>40082</v>
       </c>
       <c r="B45" s="1">
-        <v>39.062260000000002</v>
+        <v>36.138522999999999</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
@@ -728,7 +728,7 @@
         <v>40084</v>
       </c>
       <c r="B46" s="1">
-        <v>57.423400000000001</v>
+        <v>52.828957000000003</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -736,7 +736,7 @@
         <v>40085</v>
       </c>
       <c r="B47" s="1">
-        <v>47.065776999999997</v>
+        <v>52.654130000000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
@@ -744,7 +744,7 @@
         <v>40088</v>
       </c>
       <c r="B48" s="1">
-        <v>32.000459999999997</v>
+        <v>37.944476999999999</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -752,7 +752,7 @@
         <v>40089</v>
       </c>
       <c r="B49" s="1">
-        <v>49.346836000000003</v>
+        <v>45.219917000000002</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -760,7 +760,7 @@
         <v>40092</v>
       </c>
       <c r="B50" s="1">
-        <v>47.777054</v>
+        <v>44.63306</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -768,7 +768,7 @@
         <v>40094</v>
       </c>
       <c r="B51" s="1">
-        <v>43.703330000000001</v>
+        <v>45.073962999999999</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
@@ -776,7 +776,7 @@
         <v>40096</v>
       </c>
       <c r="B52" s="1">
-        <v>44.327970000000001</v>
+        <v>39.933743</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -784,7 +784,7 @@
         <v>40097</v>
       </c>
       <c r="B53" s="1">
-        <v>41.65128</v>
+        <v>37.178420000000003</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
@@ -792,7 +792,7 @@
         <v>40098</v>
       </c>
       <c r="B54" s="1">
-        <v>39.841200000000001</v>
+        <v>45.636054999999999</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
@@ -800,7 +800,7 @@
         <v>40099</v>
       </c>
       <c r="B55" s="1">
-        <v>37.691372000000001</v>
+        <v>41.213290000000001</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
@@ -808,7 +808,7 @@
         <v>40100</v>
       </c>
       <c r="B56" s="1">
-        <v>42.428885999999999</v>
+        <v>43.66507</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
@@ -816,7 +816,7 @@
         <v>40101</v>
       </c>
       <c r="B57" s="1">
-        <v>46.658546000000001</v>
+        <v>47.574905000000001</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -824,7 +824,7 @@
         <v>40103</v>
       </c>
       <c r="B58" s="1">
-        <v>44.222324</v>
+        <v>31.628167999999999</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -832,7 +832,7 @@
         <v>40105</v>
       </c>
       <c r="B59" s="1">
-        <v>42.057358000000001</v>
+        <v>50.437427999999997</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
@@ -840,7 +840,7 @@
         <v>40106</v>
       </c>
       <c r="B60" s="1">
-        <v>37.125664</v>
+        <v>42.888893000000003</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
@@ -848,7 +848,7 @@
         <v>40108</v>
       </c>
       <c r="B61" s="1">
-        <v>36.796039999999998</v>
+        <v>42.397537</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -856,7 +856,7 @@
         <v>40109</v>
       </c>
       <c r="B62" s="1">
-        <v>40.521410000000003</v>
+        <v>47.927599999999998</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
@@ -864,7 +864,7 @@
         <v>40110</v>
       </c>
       <c r="B63" s="1">
-        <v>36.129401999999999</v>
+        <v>43.809401999999999</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -872,7 +872,7 @@
         <v>40112</v>
       </c>
       <c r="B64" s="1">
-        <v>50.335106000000003</v>
+        <v>46.535310000000003</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
@@ -880,7 +880,7 @@
         <v>40117</v>
       </c>
       <c r="B65" s="1">
-        <v>35.971622000000004</v>
+        <v>45.733800000000002</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
@@ -888,7 +888,7 @@
         <v>40122</v>
       </c>
       <c r="B66" s="1">
-        <v>37.208717</v>
+        <v>40.984406</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -896,7 +896,7 @@
         <v>40126</v>
       </c>
       <c r="B67" s="1">
-        <v>41.065967999999998</v>
+        <v>38.535620000000002</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -904,7 +904,7 @@
         <v>40132</v>
       </c>
       <c r="B68" s="1">
-        <v>53.893196000000003</v>
+        <v>39.898569999999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
@@ -912,7 +912,7 @@
         <v>40133</v>
       </c>
       <c r="B69" s="1">
-        <v>45.107104999999997</v>
+        <v>46.461243000000003</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
@@ -920,7 +920,7 @@
         <v>40137</v>
       </c>
       <c r="B70" s="1">
-        <v>41.463805999999998</v>
+        <v>45.819369999999999</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
@@ -928,7 +928,7 @@
         <v>40142</v>
       </c>
       <c r="B71" s="1">
-        <v>41.921191999999998</v>
+        <v>36.224193999999997</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.4">
@@ -936,7 +936,7 @@
         <v>40143</v>
       </c>
       <c r="B72" s="1">
-        <v>43.506070000000001</v>
+        <v>45.800190000000001</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.4">
@@ -944,7 +944,7 @@
         <v>40145</v>
       </c>
       <c r="B73" s="1">
-        <v>39.308666000000002</v>
+        <v>41.541041999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>